<commit_message>
Update maps to Legion atalas
</commit_message>
<xml_diff>
--- a/PoEMapsModel/Maps/MapList/MapList.xlsx
+++ b/PoEMapsModel/Maps/MapList/MapList.xlsx
@@ -1,29 +1,34 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="21601"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="21629"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Google Drive\Personal\C#\PoeMaps\PoEMaps\MapList\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AA061FF9-5390-4A7B-A3BE-58A6870A2C27}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F279142F-AFAA-4354-AD10-41D0357A5D76}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="MapList" sheetId="1" r:id="rId1"/>
+    <sheet name="Synthesis" sheetId="1" r:id="rId1"/>
+    <sheet name="Legion" sheetId="2" r:id="rId2"/>
   </sheets>
+  <externalReferences>
+    <externalReference r:id="rId3"/>
+  </externalReferences>
   <definedNames>
-    <definedName name="MapList">MapList!$A$1:$B$158</definedName>
+    <definedName name="MapList" localSheetId="1">#REF!</definedName>
+    <definedName name="MapList">Synthesis!$A$1:$B$158</definedName>
   </definedNames>
   <calcPr calcId="125725"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="251" uniqueCount="251">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="503" uniqueCount="261">
   <si>
     <t>The Coward's Trial</t>
   </si>
@@ -776,6 +781,36 @@
   </si>
   <si>
     <t>Shaped Wharf Map</t>
+  </si>
+  <si>
+    <t>The Hall of Grandmasters</t>
+  </si>
+  <si>
+    <t>Shaped Ivory Temple Map</t>
+  </si>
+  <si>
+    <t>Perandus Manor</t>
+  </si>
+  <si>
+    <t>Oba's Cursed Trove</t>
+  </si>
+  <si>
+    <t>Shaped Waste Pool Map</t>
+  </si>
+  <si>
+    <t>Shaped Arena Map</t>
+  </si>
+  <si>
+    <t>Shaped Racecourse Map</t>
+  </si>
+  <si>
+    <t>Shaped Arsenal Map</t>
+  </si>
+  <si>
+    <t>Desert Springs Map</t>
+  </si>
+  <si>
+    <t>Shaped Bog Map</t>
   </si>
 </sst>
 </file>
@@ -828,6 +863,19 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/externalLinks/externalLink1.xml><?xml version="1.0" encoding="utf-8"?>
+<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
+  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
+    <sheetNames>
+      <sheetName val="Legion"/>
+    </sheetNames>
+    <sheetDataSet>
+      <sheetData sheetId="0" refreshError="1"/>
+    </sheetDataSet>
+  </externalBook>
+</externalLink>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1154,7 +1202,7 @@
   <dimension ref="A1:B251"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A203" sqref="A203:XFD203"/>
+      <selection activeCell="G11" sqref="G11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3176,4 +3224,2039 @@
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{95D4F90D-84A9-47DB-A1F5-39DAEB66C67B}">
+  <dimension ref="A1:B252"/>
+  <sheetViews>
+    <sheetView topLeftCell="A175" workbookViewId="0">
+      <selection activeCell="E173" sqref="E173"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="26.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="3" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>48</v>
+      </c>
+      <c r="B1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>26</v>
+      </c>
+      <c r="B2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>31</v>
+      </c>
+      <c r="B3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>140</v>
+      </c>
+      <c r="B4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>45</v>
+      </c>
+      <c r="B5">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>54</v>
+      </c>
+      <c r="B6">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>20</v>
+      </c>
+      <c r="B7">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>43</v>
+      </c>
+      <c r="B8">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>35</v>
+      </c>
+      <c r="B9">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>42</v>
+      </c>
+      <c r="B10">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>30</v>
+      </c>
+      <c r="B11">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>38</v>
+      </c>
+      <c r="B12">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>29</v>
+      </c>
+      <c r="B13">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>107</v>
+      </c>
+      <c r="B14">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>76</v>
+      </c>
+      <c r="B15">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>28</v>
+      </c>
+      <c r="B16">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>82</v>
+      </c>
+      <c r="B17">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>40</v>
+      </c>
+      <c r="B18">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>111</v>
+      </c>
+      <c r="B19">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>53</v>
+      </c>
+      <c r="B20">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>25</v>
+      </c>
+      <c r="B21">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>56</v>
+      </c>
+      <c r="B22">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>44</v>
+      </c>
+      <c r="B23">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>70</v>
+      </c>
+      <c r="B24">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>55</v>
+      </c>
+      <c r="B25">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>50</v>
+      </c>
+      <c r="B26">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>18</v>
+      </c>
+      <c r="B27">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>23</v>
+      </c>
+      <c r="B28">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>37</v>
+      </c>
+      <c r="B29">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>41</v>
+      </c>
+      <c r="B30">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>0</v>
+      </c>
+      <c r="B31">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>1</v>
+      </c>
+      <c r="B32">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>49</v>
+      </c>
+      <c r="B33">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>36</v>
+      </c>
+      <c r="B34">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
+        <v>97</v>
+      </c>
+      <c r="B35">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
+        <v>22</v>
+      </c>
+      <c r="B36">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
+        <v>59</v>
+      </c>
+      <c r="B37">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
+        <v>102</v>
+      </c>
+      <c r="B38">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A39" t="s">
+        <v>32</v>
+      </c>
+      <c r="B39">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A40" t="s">
+        <v>24</v>
+      </c>
+      <c r="B40">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A41" t="s">
+        <v>46</v>
+      </c>
+      <c r="B41">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="42" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A42" t="s">
+        <v>19</v>
+      </c>
+      <c r="B42">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="43" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A43" t="s">
+        <v>78</v>
+      </c>
+      <c r="B43">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="44" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A44" t="s">
+        <v>51</v>
+      </c>
+      <c r="B44">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="45" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A45" t="s">
+        <v>52</v>
+      </c>
+      <c r="B45">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="46" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A46" t="s">
+        <v>33</v>
+      </c>
+      <c r="B46">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="47" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A47" t="s">
+        <v>34</v>
+      </c>
+      <c r="B47">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="48" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A48" t="s">
+        <v>61</v>
+      </c>
+      <c r="B48">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="49" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A49" t="s">
+        <v>101</v>
+      </c>
+      <c r="B49">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="50" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A50" t="s">
+        <v>89</v>
+      </c>
+      <c r="B50">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="51" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A51" t="s">
+        <v>151</v>
+      </c>
+      <c r="B51">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="52" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A52" t="s">
+        <v>110</v>
+      </c>
+      <c r="B52">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="53" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A53" t="s">
+        <v>67</v>
+      </c>
+      <c r="B53">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="54" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A54" t="s">
+        <v>3</v>
+      </c>
+      <c r="B54">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="55" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A55" t="s">
+        <v>251</v>
+      </c>
+      <c r="B55">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="56" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A56" t="s">
+        <v>2</v>
+      </c>
+      <c r="B56">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="57" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A57" t="s">
+        <v>4</v>
+      </c>
+      <c r="B57">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="58" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A58" t="s">
+        <v>187</v>
+      </c>
+      <c r="B58">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="59" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A59" t="s">
+        <v>165</v>
+      </c>
+      <c r="B59">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="60" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A60" t="s">
+        <v>170</v>
+      </c>
+      <c r="B60">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="61" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A61" t="s">
+        <v>252</v>
+      </c>
+      <c r="B61">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="62" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A62" t="s">
+        <v>63</v>
+      </c>
+      <c r="B62">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="63" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A63" t="s">
+        <v>72</v>
+      </c>
+      <c r="B63">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="64" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A64" t="s">
+        <v>114</v>
+      </c>
+      <c r="B64">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="65" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A65" t="s">
+        <v>27</v>
+      </c>
+      <c r="B65">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="66" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A66" t="s">
+        <v>146</v>
+      </c>
+      <c r="B66">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="67" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A67" t="s">
+        <v>57</v>
+      </c>
+      <c r="B67">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="68" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A68" t="s">
+        <v>64</v>
+      </c>
+      <c r="B68">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="69" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A69" t="s">
+        <v>80</v>
+      </c>
+      <c r="B69">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="70" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A70" t="s">
+        <v>83</v>
+      </c>
+      <c r="B70">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="71" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A71" t="s">
+        <v>92</v>
+      </c>
+      <c r="B71">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="72" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A72" t="s">
+        <v>65</v>
+      </c>
+      <c r="B72">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="73" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A73" t="s">
+        <v>7</v>
+      </c>
+      <c r="B73">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="74" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A74" t="s">
+        <v>184</v>
+      </c>
+      <c r="B74">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="75" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A75" t="s">
+        <v>193</v>
+      </c>
+      <c r="B75">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="76" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A76" t="s">
+        <v>159</v>
+      </c>
+      <c r="B76">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="77" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A77" t="s">
+        <v>182</v>
+      </c>
+      <c r="B77">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="78" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A78" t="s">
+        <v>174</v>
+      </c>
+      <c r="B78">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="79" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A79" t="s">
+        <v>181</v>
+      </c>
+      <c r="B79">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="80" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A80" t="s">
+        <v>21</v>
+      </c>
+      <c r="B80">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="81" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A81" t="s">
+        <v>68</v>
+      </c>
+      <c r="B81">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="82" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A82" t="s">
+        <v>71</v>
+      </c>
+      <c r="B82">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="83" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A83" t="s">
+        <v>79</v>
+      </c>
+      <c r="B83">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="84" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A84" t="s">
+        <v>106</v>
+      </c>
+      <c r="B84">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="85" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A85" t="s">
+        <v>86</v>
+      </c>
+      <c r="B85">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="86" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A86" t="s">
+        <v>108</v>
+      </c>
+      <c r="B86">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="87" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A87" t="s">
+        <v>81</v>
+      </c>
+      <c r="B87">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="88" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A88" t="s">
+        <v>104</v>
+      </c>
+      <c r="B88">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="89" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A89" t="s">
+        <v>66</v>
+      </c>
+      <c r="B89">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="90" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A90" t="s">
+        <v>74</v>
+      </c>
+      <c r="B90">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="91" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A91" t="s">
+        <v>9</v>
+      </c>
+      <c r="B91">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="92" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A92" t="s">
+        <v>253</v>
+      </c>
+      <c r="B92">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="93" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A93" t="s">
+        <v>10</v>
+      </c>
+      <c r="B93">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="94" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A94" t="s">
+        <v>5</v>
+      </c>
+      <c r="B94">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="95" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A95" t="s">
+        <v>169</v>
+      </c>
+      <c r="B95">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="96" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A96" t="s">
+        <v>177</v>
+      </c>
+      <c r="B96">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="97" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A97" t="s">
+        <v>168</v>
+      </c>
+      <c r="B97">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="98" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A98" t="s">
+        <v>246</v>
+      </c>
+      <c r="B98">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="99" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A99" t="s">
+        <v>215</v>
+      </c>
+      <c r="B99">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="100" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A100" t="s">
+        <v>167</v>
+      </c>
+      <c r="B100">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="101" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A101" t="s">
+        <v>221</v>
+      </c>
+      <c r="B101">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="102" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A102" t="s">
+        <v>179</v>
+      </c>
+      <c r="B102">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="103" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A103" t="s">
+        <v>250</v>
+      </c>
+      <c r="B103">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="104" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A104" t="s">
+        <v>192</v>
+      </c>
+      <c r="B104">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="105" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A105" t="s">
+        <v>103</v>
+      </c>
+      <c r="B105">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="106" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A106" t="s">
+        <v>39</v>
+      </c>
+      <c r="B106">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="107" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A107" t="s">
+        <v>93</v>
+      </c>
+      <c r="B107">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="108" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A108" t="s">
+        <v>73</v>
+      </c>
+      <c r="B108">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="109" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A109" t="s">
+        <v>99</v>
+      </c>
+      <c r="B109">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="110" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A110" t="s">
+        <v>47</v>
+      </c>
+      <c r="B110">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="111" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A111" t="s">
+        <v>95</v>
+      </c>
+      <c r="B111">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="112" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A112" t="s">
+        <v>77</v>
+      </c>
+      <c r="B112">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="113" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A113" t="s">
+        <v>105</v>
+      </c>
+      <c r="B113">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="114" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A114" t="s">
+        <v>119</v>
+      </c>
+      <c r="B114">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="115" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A115" t="s">
+        <v>88</v>
+      </c>
+      <c r="B115">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="116" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A116" t="s">
+        <v>8</v>
+      </c>
+      <c r="B116">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="117" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A117" t="s">
+        <v>16</v>
+      </c>
+      <c r="B117">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="118" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A118" t="s">
+        <v>14</v>
+      </c>
+      <c r="B118">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="119" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A119" t="s">
+        <v>254</v>
+      </c>
+      <c r="B119">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="120" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A120" t="s">
+        <v>164</v>
+      </c>
+      <c r="B120">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="121" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A121" t="s">
+        <v>195</v>
+      </c>
+      <c r="B121">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="122" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A122" t="s">
+        <v>183</v>
+      </c>
+      <c r="B122">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="123" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A123" t="s">
+        <v>209</v>
+      </c>
+      <c r="B123">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="124" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A124" t="s">
+        <v>194</v>
+      </c>
+      <c r="B124">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="125" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A125" t="s">
+        <v>189</v>
+      </c>
+      <c r="B125">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="126" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A126" t="s">
+        <v>157</v>
+      </c>
+      <c r="B126">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="127" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A127" t="s">
+        <v>162</v>
+      </c>
+      <c r="B127">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="128" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A128" t="s">
+        <v>176</v>
+      </c>
+      <c r="B128">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="129" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A129" t="s">
+        <v>180</v>
+      </c>
+      <c r="B129">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="130" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A130" t="s">
+        <v>60</v>
+      </c>
+      <c r="B130">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="131" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A131" t="s">
+        <v>100</v>
+      </c>
+      <c r="B131">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="132" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A132" t="s">
+        <v>90</v>
+      </c>
+      <c r="B132">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="133" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A133" t="s">
+        <v>62</v>
+      </c>
+      <c r="B133">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="134" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A134" t="s">
+        <v>120</v>
+      </c>
+      <c r="B134">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="135" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A135" t="s">
+        <v>109</v>
+      </c>
+      <c r="B135">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="136" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A136" t="s">
+        <v>87</v>
+      </c>
+      <c r="B136">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="137" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A137" t="s">
+        <v>69</v>
+      </c>
+      <c r="B137">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="138" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A138" t="s">
+        <v>75</v>
+      </c>
+      <c r="B138">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="139" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A139" t="s">
+        <v>94</v>
+      </c>
+      <c r="B139">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="140" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A140" t="s">
+        <v>12</v>
+      </c>
+      <c r="B140">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="141" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A141" t="s">
+        <v>188</v>
+      </c>
+      <c r="B141">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="142" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A142" t="s">
+        <v>175</v>
+      </c>
+      <c r="B142">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="143" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A143" t="s">
+        <v>236</v>
+      </c>
+      <c r="B143">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="144" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A144" t="s">
+        <v>161</v>
+      </c>
+      <c r="B144">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="145" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A145" t="s">
+        <v>198</v>
+      </c>
+      <c r="B145">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="146" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A146" t="s">
+        <v>241</v>
+      </c>
+      <c r="B146">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="147" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A147" t="s">
+        <v>171</v>
+      </c>
+      <c r="B147">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="148" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A148" t="s">
+        <v>163</v>
+      </c>
+      <c r="B148">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="149" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A149" t="s">
+        <v>185</v>
+      </c>
+      <c r="B149">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="150" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A150" t="s">
+        <v>158</v>
+      </c>
+      <c r="B150">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="151" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A151" t="s">
+        <v>121</v>
+      </c>
+      <c r="B151">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="152" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A152" t="s">
+        <v>117</v>
+      </c>
+      <c r="B152">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="153" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A153" t="s">
+        <v>58</v>
+      </c>
+      <c r="B153">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="154" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A154" t="s">
+        <v>122</v>
+      </c>
+      <c r="B154">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="155" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A155" t="s">
+        <v>137</v>
+      </c>
+      <c r="B155">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="156" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A156" t="s">
+        <v>136</v>
+      </c>
+      <c r="B156">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="157" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A157" t="s">
+        <v>133</v>
+      </c>
+      <c r="B157">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="158" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A158" t="s">
+        <v>124</v>
+      </c>
+      <c r="B158">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="159" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A159" t="s">
+        <v>139</v>
+      </c>
+      <c r="B159">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="160" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A160" t="s">
+        <v>91</v>
+      </c>
+      <c r="B160">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="161" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A161" t="s">
+        <v>15</v>
+      </c>
+      <c r="B161">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="162" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A162" t="s">
+        <v>217</v>
+      </c>
+      <c r="B162">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="163" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A163" t="s">
+        <v>190</v>
+      </c>
+      <c r="B163">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="164" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A164" t="s">
+        <v>191</v>
+      </c>
+      <c r="B164">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="165" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A165" t="s">
+        <v>172</v>
+      </c>
+      <c r="B165">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="166" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A166" t="s">
+        <v>173</v>
+      </c>
+      <c r="B166">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="167" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A167" t="s">
+        <v>200</v>
+      </c>
+      <c r="B167">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="168" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A168" t="s">
+        <v>240</v>
+      </c>
+      <c r="B168">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="169" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A169" t="s">
+        <v>228</v>
+      </c>
+      <c r="B169">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="170" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A170" t="s">
+        <v>255</v>
+      </c>
+      <c r="B170">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="171" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A171" t="s">
+        <v>249</v>
+      </c>
+      <c r="B171">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="172" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A172" t="s">
+        <v>206</v>
+      </c>
+      <c r="B172">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="173" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A173" t="s">
+        <v>147</v>
+      </c>
+      <c r="B173">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="174" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A174" t="s">
+        <v>85</v>
+      </c>
+      <c r="B174">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="175" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A175" t="s">
+        <v>98</v>
+      </c>
+      <c r="B175">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="176" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A176" t="s">
+        <v>135</v>
+      </c>
+      <c r="B176">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="177" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A177" t="s">
+        <v>138</v>
+      </c>
+      <c r="B177">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="178" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A178" t="s">
+        <v>148</v>
+      </c>
+      <c r="B178">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="179" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A179" t="s">
+        <v>129</v>
+      </c>
+      <c r="B179">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="180" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A180" t="s">
+        <v>96</v>
+      </c>
+      <c r="B180">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="181" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A181" t="s">
+        <v>134</v>
+      </c>
+      <c r="B181">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="182" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A182" t="s">
+        <v>11</v>
+      </c>
+      <c r="B182">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="183" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A183" t="s">
+        <v>13</v>
+      </c>
+      <c r="B183">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="184" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A184" t="s">
+        <v>202</v>
+      </c>
+      <c r="B184">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="185" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A185" t="s">
+        <v>211</v>
+      </c>
+      <c r="B185">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="186" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A186" t="s">
+        <v>256</v>
+      </c>
+      <c r="B186">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="187" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A187" t="s">
+        <v>166</v>
+      </c>
+      <c r="B187">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="188" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A188" t="s">
+        <v>257</v>
+      </c>
+      <c r="B188">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="189" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A189" t="s">
+        <v>196</v>
+      </c>
+      <c r="B189">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="190" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A190" t="s">
+        <v>203</v>
+      </c>
+      <c r="B190">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="191" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A191" t="s">
+        <v>219</v>
+      </c>
+      <c r="B191">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="192" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A192" t="s">
+        <v>222</v>
+      </c>
+      <c r="B192">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="193" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A193" t="s">
+        <v>231</v>
+      </c>
+      <c r="B193">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="194" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A194" t="s">
+        <v>204</v>
+      </c>
+      <c r="B194">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="195" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A195" t="s">
+        <v>132</v>
+      </c>
+      <c r="B195">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="196" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A196" t="s">
+        <v>126</v>
+      </c>
+      <c r="B196">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="197" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A197" t="s">
+        <v>149</v>
+      </c>
+      <c r="B197">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="198" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A198" t="s">
+        <v>141</v>
+      </c>
+      <c r="B198">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="199" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A199" t="s">
+        <v>118</v>
+      </c>
+      <c r="B199">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="200" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A200" t="s">
+        <v>142</v>
+      </c>
+      <c r="B200">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="201" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A201" t="s">
+        <v>144</v>
+      </c>
+      <c r="B201">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="202" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A202" t="s">
+        <v>130</v>
+      </c>
+      <c r="B202">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="203" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A203" t="s">
+        <v>123</v>
+      </c>
+      <c r="B203">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="204" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A204" t="s">
+        <v>160</v>
+      </c>
+      <c r="B204">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="205" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A205" t="s">
+        <v>207</v>
+      </c>
+      <c r="B205">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="206" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A206" t="s">
+        <v>210</v>
+      </c>
+      <c r="B206">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="207" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A207" t="s">
+        <v>218</v>
+      </c>
+      <c r="B207">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="208" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A208" t="s">
+        <v>245</v>
+      </c>
+      <c r="B208">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="209" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A209" t="s">
+        <v>225</v>
+      </c>
+      <c r="B209">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="210" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A210" t="s">
+        <v>247</v>
+      </c>
+      <c r="B210">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="211" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A211" t="s">
+        <v>220</v>
+      </c>
+      <c r="B211">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="212" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A212" t="s">
+        <v>243</v>
+      </c>
+      <c r="B212">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="213" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A213" t="s">
+        <v>205</v>
+      </c>
+      <c r="B213">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="214" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A214" t="s">
+        <v>213</v>
+      </c>
+      <c r="B214">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="215" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A215" t="s">
+        <v>145</v>
+      </c>
+      <c r="B215">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="216" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A216" t="s">
+        <v>84</v>
+      </c>
+      <c r="B216">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="217" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A217" t="s">
+        <v>113</v>
+      </c>
+      <c r="B217">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="218" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A218" t="s">
+        <v>127</v>
+      </c>
+      <c r="B218">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="219" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A219" t="s">
+        <v>125</v>
+      </c>
+      <c r="B219">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="220" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A220" t="s">
+        <v>112</v>
+      </c>
+      <c r="B220">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="221" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A221" t="s">
+        <v>150</v>
+      </c>
+      <c r="B221">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="222" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A222" t="s">
+        <v>242</v>
+      </c>
+      <c r="B222">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="223" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A223" t="s">
+        <v>178</v>
+      </c>
+      <c r="B223">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="224" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A224" t="s">
+        <v>232</v>
+      </c>
+      <c r="B224">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="225" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A225" t="s">
+        <v>212</v>
+      </c>
+      <c r="B225">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="226" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A226" t="s">
+        <v>238</v>
+      </c>
+      <c r="B226">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="227" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A227" t="s">
+        <v>186</v>
+      </c>
+      <c r="B227">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="228" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A228" t="s">
+        <v>234</v>
+      </c>
+      <c r="B228">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="229" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A229" t="s">
+        <v>216</v>
+      </c>
+      <c r="B229">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="230" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A230" t="s">
+        <v>244</v>
+      </c>
+      <c r="B230">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="231" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A231" t="s">
+        <v>258</v>
+      </c>
+      <c r="B231">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="232" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A232" t="s">
+        <v>227</v>
+      </c>
+      <c r="B232">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="233" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A233" t="s">
+        <v>131</v>
+      </c>
+      <c r="B233">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="234" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A234" t="s">
+        <v>143</v>
+      </c>
+      <c r="B234">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="235" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A235" t="s">
+        <v>128</v>
+      </c>
+      <c r="B235">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="236" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A236" t="s">
+        <v>259</v>
+      </c>
+      <c r="B236">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="237" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A237" t="s">
+        <v>115</v>
+      </c>
+      <c r="B237">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="238" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A238" t="s">
+        <v>199</v>
+      </c>
+      <c r="B238">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="239" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A239" t="s">
+        <v>239</v>
+      </c>
+      <c r="B239">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="240" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A240" t="s">
+        <v>229</v>
+      </c>
+      <c r="B240">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="241" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A241" t="s">
+        <v>201</v>
+      </c>
+      <c r="B241">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="242" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A242" t="s">
+        <v>260</v>
+      </c>
+      <c r="B242">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="243" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A243" t="s">
+        <v>248</v>
+      </c>
+      <c r="B243">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="244" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A244" t="s">
+        <v>226</v>
+      </c>
+      <c r="B244">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="245" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A245" t="s">
+        <v>208</v>
+      </c>
+      <c r="B245">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="246" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A246" t="s">
+        <v>214</v>
+      </c>
+      <c r="B246">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="247" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A247" t="s">
+        <v>233</v>
+      </c>
+      <c r="B247">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="248" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A248" t="s">
+        <v>156</v>
+      </c>
+      <c r="B248">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="249" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A249" t="s">
+        <v>155</v>
+      </c>
+      <c r="B249">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="250" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A250" t="s">
+        <v>154</v>
+      </c>
+      <c r="B250">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="251" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A251" t="s">
+        <v>152</v>
+      </c>
+      <c r="B251">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="252" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A252" t="s">
+        <v>153</v>
+      </c>
+      <c r="B252">
+        <v>16</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>